<commit_message>
Preprocessing edited to extract and save faces
</commit_message>
<xml_diff>
--- a/output/results.xlsx
+++ b/output/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edward Sims\Documents\ml_projects\nerdycat\deepfake-detection-challenge\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9A786FF-4202-4D44-8608-A2D112352156}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0584E990-B74E-47E3-A438-28567FFB6076}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7BC4A8F2-1695-448B-885E-62DB5D028A6E}"/>
   </bookViews>
@@ -28,6 +28,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>cv</t>
+  </si>
+  <si>
+    <t>lb</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,12 +391,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB04594-09AC-411C-81E6-54B319E17597}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>